<commit_message>
Daily updates. Schematic done, board mostly done
</commit_message>
<xml_diff>
--- a/H2_v4/BOM.xlsx
+++ b/H2_v4/BOM.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Digikey part #</t>
   </si>
@@ -49,6 +49,72 @@
   </si>
   <si>
     <t>Small NFET</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LTC7001EMSE#PBF-ND</t>
+  </si>
+  <si>
+    <t>High side driver</t>
+  </si>
+  <si>
+    <t>102-4244-ND</t>
+  </si>
+  <si>
+    <t>5v Buck converter</t>
+  </si>
+  <si>
+    <t>1568-1233-ND</t>
+  </si>
+  <si>
+    <t>Teensy</t>
+  </si>
+  <si>
+    <t>565-3816-ND</t>
+  </si>
+  <si>
+    <t>Aluminum capacitor</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Button pad</t>
+  </si>
+  <si>
+    <t>Supercaps</t>
+  </si>
+  <si>
+    <t>1182-1018-ND</t>
+  </si>
+  <si>
+    <t>TPHR6503PLL1QCT-ND</t>
+  </si>
+  <si>
+    <t>Pass/short transistor</t>
+  </si>
+  <si>
+    <t>1655-1928-1-ND</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>200mOhm resistor</t>
+  </si>
+  <si>
+    <t>1276-6171-1-ND</t>
+  </si>
+  <si>
+    <t>4.7k resistor</t>
+  </si>
+  <si>
+    <t>RMCF0603JT4K70CT-ND</t>
+  </si>
+  <si>
+    <t>587-2484-1-ND</t>
+  </si>
+  <si>
+    <t>10uF cap</t>
   </si>
 </sst>
 </file>
@@ -366,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -378,7 +444,7 @@
     <col min="2" max="3" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -391,8 +457,15 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1">
+        <f>SUM(E2:E100)</f>
+        <v>52.49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -405,8 +478,12 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <f>D2*C2</f>
+        <v>16.190000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -419,8 +496,12 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <f t="shared" ref="E3:E28" si="0">D3*C3</f>
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -432,6 +513,271 @@
       </c>
       <c r="D4">
         <v>4</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>5.13</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>5.13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>2.78</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>14.38</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>14.38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>4.68</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>2.09</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>4.18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>0.18</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16">
+        <v>0.2</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17">
+        <v>0.01</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <v>0.2</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>